<commit_message>
try oht seq + random key
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuyulu\Documents\thesis\HRC_taskAlloc_w.TB_w.AR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068B303F-A624-4465-BD71-ED406FA857E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDBBDE9-CEE3-4264-BBB9-E6BF630484FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="8130" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16080" yWindow="8130" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Position" sheetId="1" r:id="rId1"/>
     <sheet name="Therbligs(L)" sheetId="3" r:id="rId2"/>
     <sheet name="Therbligs(R)" sheetId="4" r:id="rId3"/>
     <sheet name="Therblig Process Time" sheetId="5" r:id="rId4"/>
+    <sheet name="OHT Relation" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="78">
   <si>
     <t>From</t>
   </si>
@@ -287,6 +288,10 @@
   </si>
   <si>
     <t>BottomPlate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OHT_id</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1095,7 +1100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59CF949-7256-4B60-BD47-05AF650B0ADA}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
@@ -1853,4 +1858,77 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178C5327-6E4A-4907-8A11-8CF589BF8A11}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>-1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finish gantt chart, rk evolution
TODO: Bind Relation
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuyulu\Documents\thesis\HRC_taskAlloc_w.TB_w.AR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7663AA0-89F2-4C4F-8FE4-2EC26761E1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE76AE9-8AFD-4DB0-8DF6-2D9A53703B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="8130" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16080" yWindow="8130" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Position" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="79">
   <si>
     <t>From</t>
   </si>
@@ -838,10 +838,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A10" sqref="A10:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -968,6 +968,82 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -979,10 +1055,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1093,7 +1169,72 @@
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1104,7 +1245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59CF949-7256-4B60-BD47-05AF650B0ADA}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -1881,15 +2022,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178C5327-6E4A-4907-8A11-8CF589BF8A11}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -1905,8 +2046,17 @@
       <c r="E1">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1922,8 +2072,17 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1934,13 +2093,22 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1948,16 +2116,25 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1965,12 +2142,99 @@
         <v>0</v>
       </c>
       <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>-1</v>
       </c>
-      <c r="D5">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>-1</v>
       </c>
-      <c r="E5">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>-1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>-1</v>
+      </c>
+      <c r="G8">
+        <v>-1</v>
+      </c>
+      <c r="H8">
         <v>0</v>
       </c>
     </row>

</xml_diff>